<commit_message>
Oldal a loginnek, jobb nav
</commit_message>
<xml_diff>
--- a/Követelmények.xlsx
+++ b/Követelmények.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Web-design-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FD2B05-B684-4901-B1A9-0357A264C3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B946E4FF-5B25-43C2-BBB7-75D3A23569F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14925" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>Formai követelmények</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>IGEN (B)</t>
+  </si>
+  <si>
+    <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>Még több kell.</t>
   </si>
 </sst>
 </file>
@@ -403,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -673,11 +679,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -726,6 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1006,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1038,7 @@
     <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -1031,8 +1049,11 @@
       <c r="D1" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>61</v>
       </c>
@@ -1044,7 +1065,7 @@
       </c>
       <c r="D2" s="31"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1056,7 +1077,7 @@
       </c>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1068,7 +1089,7 @@
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3.1</v>
       </c>
@@ -1082,7 +1103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3.2</v>
       </c>
@@ -1094,7 +1115,7 @@
       </c>
       <c r="D6" s="33"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -1104,7 +1125,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="32"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>4.0999999999999996</v>
       </c>
@@ -1116,7 +1137,7 @@
       </c>
       <c r="D8" s="33"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>4.2</v>
       </c>
@@ -1128,7 +1149,7 @@
       </c>
       <c r="D9" s="33"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1161,7 @@
       </c>
       <c r="D10" s="34"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1173,7 @@
       </c>
       <c r="D11" s="34"/>
     </row>
-    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>4.3</v>
       </c>
@@ -1164,7 +1185,7 @@
       </c>
       <c r="D12" s="33"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -1176,7 +1197,7 @@
       </c>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>5</v>
       </c>
@@ -1188,7 +1209,7 @@
       </c>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -1198,9 +1219,11 @@
       <c r="C15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="33"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>5.2</v>
       </c>
@@ -1214,7 +1237,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>17</v>
       </c>
@@ -1228,7 +1251,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
@@ -1242,7 +1265,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>20</v>
       </c>
@@ -1256,7 +1279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>6</v>
       </c>
@@ -1268,7 +1291,7 @@
       </c>
       <c r="D20" s="36"/>
     </row>
-    <row r="21" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>6.1</v>
       </c>
@@ -1280,7 +1303,7 @@
       </c>
       <c r="D21" s="37"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>24</v>
       </c>
@@ -1290,9 +1313,14 @@
       <c r="C22" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="37"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1332,7 @@
       </c>
       <c r="D23" s="37"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>26</v>
       </c>
@@ -1316,7 +1344,7 @@
       </c>
       <c r="D24" s="37"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>27</v>
       </c>
@@ -1328,7 +1356,7 @@
       </c>
       <c r="D25" s="37"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>28</v>
       </c>
@@ -1340,7 +1368,7 @@
       </c>
       <c r="D26" s="37"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>29</v>
       </c>
@@ -1352,7 +1380,7 @@
       </c>
       <c r="D27" s="37"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1394,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>31</v>
       </c>
@@ -1380,7 +1408,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>32</v>
       </c>
@@ -1394,7 +1422,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>33</v>
       </c>
@@ -1406,7 +1434,7 @@
       </c>
       <c r="D31" s="37"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>34</v>
       </c>
@@ -1428,7 +1456,9 @@
       <c r="C33" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="38"/>
+      <c r="D33" s="38" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">

</xml_diff>

<commit_message>
Javítások, cookie Mostmár van GET adatbekérés Cookiek jól működnek, csak nincs még szinkronban Kisebb foldozások
</commit_message>
<xml_diff>
--- a/Követelmények.xlsx
+++ b/Követelmények.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Web-design-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916B72C-A4EF-4EFB-9DCC-33348B754AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDC2FD2-71DC-4EDD-9A8B-BFE495CE8D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
   <si>
     <t>Formai követelmények</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>IGEN(B)</t>
+  </si>
+  <si>
+    <t>IGEN(B) (almost)</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,7 +1350,9 @@
       <c r="C23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="37" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
@@ -1382,7 +1390,9 @@
       <c r="C26" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="37"/>
+      <c r="D26" s="37" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
@@ -1464,7 +1474,9 @@
       <c r="C32" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="37"/>
+      <c r="D32" s="37" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">

</xml_diff>